<commit_message>
End of Day 7. Mostly complete
</commit_message>
<xml_diff>
--- a/Project/weapon dps.xlsx
+++ b/Project/weapon dps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\dev\Darkside\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE89E5D8-08D7-4C09-944E-0D8158F2433A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF26EB9A-5771-450C-8770-4C52C3D830F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12030" yWindow="3630" windowWidth="12855" windowHeight="11385" xr2:uid="{9EF0D56B-EB09-438F-92CA-E96DF0AD4372}"/>
+    <workbookView xWindow="3600" yWindow="3825" windowWidth="18105" windowHeight="11385" xr2:uid="{9EF0D56B-EB09-438F-92CA-E96DF0AD4372}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Las Pistol</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>Melee</t>
   </si>
 </sst>
 </file>
@@ -436,10 +439,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{808B67BD-6A0A-4B00-9E8E-15CAEABFBDF4}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +451,7 @@
     <col min="2" max="2" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>9</v>
       </c>
@@ -465,71 +468,77 @@
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="C2">
-        <f>15/B2</f>
-        <v>60</v>
+        <f>10/B2</f>
+        <v>50</v>
       </c>
       <c r="D2">
         <f>40/B2</f>
-        <v>160</v>
+        <v>200</v>
       </c>
       <c r="E2">
-        <f>10/B2</f>
+        <f>8/B2</f>
         <v>40</v>
       </c>
       <c r="F2">
-        <f>30/B2</f>
-        <v>120</v>
+        <f>35/B2</f>
+        <v>175</v>
       </c>
       <c r="G2">
         <f>8/B2</f>
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="H2">
-        <f>20/B2</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f>25/B2</f>
+        <v>125</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="C3">
-        <f>30/B3</f>
+        <f>20/B3</f>
         <v>100</v>
       </c>
       <c r="D3">
-        <f>60/B3</f>
-        <v>200</v>
+        <f>50/B3</f>
+        <v>250</v>
       </c>
       <c r="E3">
         <f>15/B3</f>
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="F3">
-        <f>40/B3</f>
-        <v>133.33333333333334</v>
+        <f>35/B3</f>
+        <v>175</v>
       </c>
       <c r="G3">
         <f>5/B3</f>
-        <v>16.666666666666668</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <f>25/B3</f>
-        <v>83.333333333333343</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="K3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -560,104 +569,113 @@
         <f>25/B4</f>
         <v>125</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C5">
-        <f>20/B5</f>
-        <v>20</v>
+        <f>15/B5</f>
+        <v>18.75</v>
       </c>
       <c r="D5">
-        <f>70/B5</f>
-        <v>70</v>
+        <f>60/B5</f>
+        <v>75</v>
       </c>
       <c r="E5">
         <f>3/B5</f>
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="F5">
-        <f>10/B5</f>
-        <v>10</v>
+        <f>40/B5</f>
+        <v>50</v>
       </c>
       <c r="G5">
         <f>3/B5</f>
-        <v>3</v>
+        <v>3.75</v>
       </c>
       <c r="H5">
         <f>10/B5</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>12.5</v>
+      </c>
+      <c r="K5">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C6">
         <f>8*15/B6</f>
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="D6">
         <f>8*60/B6</f>
-        <v>480</v>
+        <v>600</v>
       </c>
       <c r="E6">
         <f>8*8/B6</f>
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="F6">
-        <f>8*20/B6</f>
-        <v>160</v>
+        <f>8*40/B6</f>
+        <v>400</v>
       </c>
       <c r="G6">
         <f>8*3/B6</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H6">
         <f>8*10/B6</f>
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0.3</v>
+        <v>0.25</v>
       </c>
       <c r="C7">
-        <f>45/B7</f>
-        <v>150</v>
+        <f>40/B7</f>
+        <v>160</v>
       </c>
       <c r="D7">
-        <f>70/B7</f>
-        <v>233.33333333333334</v>
+        <f>60/B7</f>
+        <v>240</v>
       </c>
       <c r="G7">
         <f>15/B7</f>
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="H7">
         <f>50/B7</f>
-        <v>166.66666666666669</v>
+        <v>200</v>
       </c>
       <c r="I7">
         <f>10/B7</f>
-        <v>33.333333333333336</v>
+        <v>40</v>
       </c>
       <c r="J7">
         <f>30/B7</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="K7">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -669,16 +687,16 @@
         <v>125</v>
       </c>
       <c r="D8">
-        <f>40/B8</f>
-        <v>200</v>
+        <f>45/B8</f>
+        <v>225</v>
       </c>
       <c r="G8">
-        <f>8/B8</f>
-        <v>40</v>
+        <f>10/B8</f>
+        <v>50</v>
       </c>
       <c r="H8">
-        <f>30/B8</f>
-        <v>150</v>
+        <f>35/B8</f>
+        <v>175</v>
       </c>
       <c r="I8">
         <f>5/B8</f>
@@ -688,40 +706,46 @@
         <f>20/B8</f>
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="C9">
-        <f>50/B9</f>
-        <v>151.5151515151515</v>
+        <f>45/B9</f>
+        <v>150</v>
       </c>
       <c r="D9">
-        <f>75/B9</f>
-        <v>227.27272727272725</v>
+        <f>70/B9</f>
+        <v>233.33333333333334</v>
       </c>
       <c r="G9">
         <f>30/B9</f>
-        <v>90.909090909090907</v>
+        <v>100</v>
       </c>
       <c r="H9">
         <f>60/B9</f>
-        <v>181.81818181818181</v>
+        <v>200</v>
       </c>
       <c r="I9">
         <f>10/B9</f>
-        <v>30.303030303030301</v>
+        <v>33.333333333333336</v>
       </c>
       <c r="J9">
         <f>30/B9</f>
-        <v>90.909090909090907</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="K9">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -729,12 +753,12 @@
         <v>1</v>
       </c>
       <c r="C10">
-        <f>145/B10</f>
-        <v>145</v>
+        <f>125/B10</f>
+        <v>125</v>
       </c>
       <c r="D10">
-        <f>250/B10</f>
-        <v>250</v>
+        <f>350/B10</f>
+        <v>350</v>
       </c>
       <c r="I10">
         <f>108/B10</f>
@@ -744,8 +768,33 @@
         <f>175/B10</f>
         <v>175</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K10">
+        <v>22</v>
+      </c>
+      <c r="L10">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0.4</v>
+      </c>
+      <c r="C11">
+        <f>100/B11</f>
+        <v>250</v>
+      </c>
+      <c r="D11">
+        <f>200/B11</f>
+        <v>500</v>
+      </c>
+      <c r="K11">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>11</v>
       </c>
@@ -756,7 +805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -770,7 +819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>100*B13</f>
         <v>200</v>

</xml_diff>

<commit_message>
ready for final testing
</commit_message>
<xml_diff>
--- a/Project/weapon dps.xlsx
+++ b/Project/weapon dps.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\dev\Darkside\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF26EB9A-5771-450C-8770-4C52C3D830F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7481B9DB-46BB-466D-B4E2-3C48BBE9C82F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3600" yWindow="3825" windowWidth="18105" windowHeight="11385" xr2:uid="{9EF0D56B-EB09-438F-92CA-E96DF0AD4372}"/>
   </bookViews>
@@ -442,7 +442,7 @@
   <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,16 +480,16 @@
         <v>50</v>
       </c>
       <c r="D2">
-        <f>40/B2</f>
-        <v>200</v>
+        <f>50/B2</f>
+        <v>250</v>
       </c>
       <c r="E2">
         <f>8/B2</f>
         <v>40</v>
       </c>
       <c r="F2">
-        <f>35/B2</f>
-        <v>175</v>
+        <f>40/B2</f>
+        <v>200</v>
       </c>
       <c r="G2">
         <f>8/B2</f>
@@ -550,16 +550,16 @@
         <v>110</v>
       </c>
       <c r="D4">
-        <f>45/B4</f>
-        <v>225</v>
+        <f>50/B4</f>
+        <v>250</v>
       </c>
       <c r="E4">
         <f>18/B4</f>
         <v>90</v>
       </c>
       <c r="F4">
-        <f>35/B4</f>
-        <v>175</v>
+        <f>40/B4</f>
+        <v>200</v>
       </c>
       <c r="I4">
         <f>10/B4</f>

</xml_diff>